<commit_message>
[MDTUDDM-28613] added deployment mode and monitoring
Change-Id: I6ef60a5db7326989af222b74e5a1a6a591f45853
</commit_message>
<xml_diff>
--- a/docs/ua/modules/arch/attachments/architecture-workspace/registry-resources.xlsx
+++ b/docs/ua/modules/arch/attachments/architecture-workspace/registry-resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Maksym_Kharchenko/Work/Development/mdtu-ddm/mdtu-ddm-gerrit-workspace/mdtu-ddm/general/ddm-architecture/docs/ua/modules/arch/attachments/architecture/platform-system-requirements/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruslan_Lesyk\Desktop\ddm-architecture\docs\ua\modules\arch\attachments\architecture-workspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1DA3E55-169F-E643-B1BC-E8FD9CF974E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7866B66D-60E5-4490-8292-4F0DBCCBB5CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="33600" windowHeight="20340" xr2:uid="{76BACE1B-BDCC-F34F-9205-7BB42BE8027F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{76BACE1B-BDCC-F34F-9205-7BB42BE8027F}"/>
   </bookViews>
   <sheets>
     <sheet name="Registry Resources" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="130">
   <si>
     <t>Technology</t>
   </si>
@@ -170,9 +170,6 @@
     <t>operational-pool</t>
   </si>
   <si>
-    <t>pdadmin-deployment</t>
-  </si>
-  <si>
     <t>platform-gateway-deployment</t>
   </si>
   <si>
@@ -417,6 +414,18 @@
   </si>
   <si>
     <t>GC (baseline)</t>
+  </si>
+  <si>
+    <t>production+development</t>
+  </si>
+  <si>
+    <t>development</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +</t>
+  </si>
+  <si>
+    <t>pgadmin-deployment</t>
   </si>
 </sst>
 </file>
@@ -612,13 +621,13 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -722,13 +731,13 @@
     <tableColumn id="7" xr3:uid="{7D3E02CE-7CDD-5E44-88DF-1162888AE695}" name="-Xms, Mb (baseline)" dataDxfId="9"/>
     <tableColumn id="8" xr3:uid="{3D28B649-AB9D-9C49-8889-6B0D4888A8D3}" name="-Xmx, Mb (baseline)" dataDxfId="8"/>
     <tableColumn id="13" xr3:uid="{729BA2AA-0236-6D4E-88FA-AF5279155852}" name="-Xmn, Mb (baseline)" dataDxfId="7"/>
-    <tableColumn id="22" xr3:uid="{4E8AEAD1-7BE7-C842-8ED6-80C30C596EB7}" name="Metaspace, Mb (baseline)" dataDxfId="1"/>
-    <tableColumn id="23" xr3:uid="{60B01E56-F1C6-2843-8907-B681700354AC}" name="GC (baseline)" dataDxfId="0"/>
-    <tableColumn id="21" xr3:uid="{0E115C8F-10F3-1849-9086-23ECFF100762}" name="-Xms, Mb (target)" dataDxfId="6"/>
-    <tableColumn id="20" xr3:uid="{59ED4565-1835-554A-B6BE-EFEE9FF75498}" name="-Xmx, Mb (target)" dataDxfId="5"/>
-    <tableColumn id="19" xr3:uid="{5B7661BC-38C4-754F-9E3A-2E5DFADC19B1}" name="-Xmn, Mb (target)" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{84FF7781-94A1-1246-98C1-52FEAF154639}" name="Java Opts (baseline)" dataDxfId="3"/>
-    <tableColumn id="18" xr3:uid="{8EF485D1-BA5B-0B42-B711-53E12FB7661E}" name="Java Opts (target)" dataDxfId="2"/>
+    <tableColumn id="22" xr3:uid="{4E8AEAD1-7BE7-C842-8ED6-80C30C596EB7}" name="Metaspace, Mb (baseline)" dataDxfId="6"/>
+    <tableColumn id="23" xr3:uid="{60B01E56-F1C6-2843-8907-B681700354AC}" name="GC (baseline)" dataDxfId="5"/>
+    <tableColumn id="21" xr3:uid="{0E115C8F-10F3-1849-9086-23ECFF100762}" name="-Xms, Mb (target)" dataDxfId="4"/>
+    <tableColumn id="20" xr3:uid="{59ED4565-1835-554A-B6BE-EFEE9FF75498}" name="-Xmx, Mb (target)" dataDxfId="3"/>
+    <tableColumn id="19" xr3:uid="{5B7661BC-38C4-754F-9E3A-2E5DFADC19B1}" name="-Xmn, Mb (target)" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{84FF7781-94A1-1246-98C1-52FEAF154639}" name="Java Opts (baseline)" dataDxfId="1"/>
+    <tableColumn id="18" xr3:uid="{8EF485D1-BA5B-0B42-B711-53E12FB7661E}" name="Java Opts (target)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1033,114 +1042,114 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C809D083-7CF6-1445-A306-E810BD791428}">
   <dimension ref="A1:W65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="R30" sqref="R30"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.83203125" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="65.83203125" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="28.796875" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="65.796875" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="35.5" customWidth="1"/>
     <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.09765625" customWidth="1"/>
+    <col min="6" max="6" width="14.296875" style="2" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="2" customWidth="1"/>
     <col min="8" max="8" width="15.5" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="18.83203125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="14.296875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="18.796875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.69921875" style="2" customWidth="1"/>
     <col min="12" max="12" width="21" style="2" customWidth="1"/>
-    <col min="13" max="13" width="21.33203125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="21.296875" style="2" customWidth="1"/>
     <col min="14" max="14" width="21.5" customWidth="1"/>
-    <col min="15" max="15" width="19.83203125" customWidth="1"/>
+    <col min="15" max="15" width="19.796875" customWidth="1"/>
     <col min="16" max="16" width="20.5" customWidth="1"/>
-    <col min="17" max="17" width="26.33203125" customWidth="1"/>
+    <col min="17" max="17" width="26.296875" customWidth="1"/>
     <col min="18" max="18" width="15.5" customWidth="1"/>
     <col min="19" max="19" width="19.5" customWidth="1"/>
-    <col min="20" max="20" width="18.1640625" customWidth="1"/>
+    <col min="20" max="20" width="18.19921875" customWidth="1"/>
     <col min="21" max="21" width="18.5" customWidth="1"/>
-    <col min="22" max="22" width="65.6640625" customWidth="1"/>
-    <col min="23" max="23" width="66.6640625" style="3" customWidth="1"/>
+    <col min="22" max="22" width="65.69921875" customWidth="1"/>
+    <col min="23" max="23" width="66.69921875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" t="s">
         <v>97</v>
-      </c>
-      <c r="H1" t="s">
-        <v>98</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="N1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>122</v>
-      </c>
       <c r="V1" t="s">
+        <v>116</v>
+      </c>
+      <c r="W1" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="W1" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:23" ht="16.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>39</v>
@@ -1148,24 +1157,28 @@
       <c r="D2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F2" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="4"/>
+      <c r="H2" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I2" s="6"/>
       <c r="J2" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L2" s="6"/>
       <c r="M2" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N2" s="4"/>
       <c r="O2" s="6"/>
@@ -1178,12 +1191,12 @@
       <c r="V2" s="4"/>
       <c r="W2" s="6"/>
     </row>
-    <row r="3" spans="1:23" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" ht="16.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>8</v>
@@ -1191,24 +1204,28 @@
       <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>127</v>
+      </c>
       <c r="F3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="4"/>
+      <c r="H3" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L3" s="6"/>
       <c r="M3" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N3" s="4"/>
       <c r="O3" s="6"/>
@@ -1221,12 +1238,12 @@
       <c r="V3" s="4"/>
       <c r="W3" s="6"/>
     </row>
-    <row r="4" spans="1:23" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" ht="16.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>11</v>
@@ -1234,24 +1251,28 @@
       <c r="D4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>127</v>
+      </c>
       <c r="F4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="4"/>
+      <c r="H4" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L4" s="6"/>
       <c r="M4" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N4" s="4"/>
       <c r="O4" s="6"/>
@@ -1264,12 +1285,12 @@
       <c r="V4" s="4"/>
       <c r="W4" s="6"/>
     </row>
-    <row r="5" spans="1:23" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" ht="16.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>14</v>
@@ -1277,24 +1298,28 @@
       <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="4"/>
+      <c r="H5" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I5" s="6"/>
       <c r="J5" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L5" s="6"/>
       <c r="M5" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="6"/>
@@ -1307,12 +1332,12 @@
       <c r="V5" s="4"/>
       <c r="W5" s="6"/>
     </row>
-    <row r="6" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>16</v>
@@ -1320,28 +1345,32 @@
       <c r="D6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F6" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="4"/>
+      <c r="H6" s="6" t="s">
+        <v>128</v>
+      </c>
       <c r="I6" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J6" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L6" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K6" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L6" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="M6" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N6" s="18">
         <v>1536</v>
@@ -1360,18 +1389,18 @@
         <v>9</v>
       </c>
       <c r="V6" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="W6" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="16.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>31</v>
@@ -1379,24 +1408,28 @@
       <c r="D7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F7" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="4"/>
+      <c r="H7" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L7" s="6"/>
       <c r="M7" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N7" s="4"/>
       <c r="O7" s="6"/>
@@ -1409,37 +1442,41 @@
       <c r="V7" s="4"/>
       <c r="W7" s="6"/>
     </row>
-    <row r="8" spans="1:23" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" ht="16.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>127</v>
+      </c>
       <c r="F8" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="4"/>
+      <c r="H8" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I8" s="6"/>
       <c r="J8" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L8" s="6"/>
       <c r="M8" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N8" s="4"/>
       <c r="O8" s="6"/>
@@ -1452,37 +1489,41 @@
       <c r="V8" s="4"/>
       <c r="W8" s="6"/>
     </row>
-    <row r="9" spans="1:23" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" ht="16.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>127</v>
+      </c>
       <c r="F9" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="4"/>
+      <c r="H9" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I9" s="6"/>
       <c r="J9" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L9" s="6"/>
       <c r="M9" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N9" s="4"/>
       <c r="O9" s="6"/>
@@ -1495,37 +1536,41 @@
       <c r="V9" s="4"/>
       <c r="W9" s="6"/>
     </row>
-    <row r="10" spans="1:23" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" ht="16.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>127</v>
+      </c>
       <c r="F10" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="4"/>
+      <c r="H10" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I10" s="6"/>
       <c r="J10" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L10" s="6"/>
       <c r="M10" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N10" s="4"/>
       <c r="O10" s="6"/>
@@ -1538,12 +1583,12 @@
       <c r="V10" s="4"/>
       <c r="W10" s="6"/>
     </row>
-    <row r="11" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>17</v>
@@ -1551,28 +1596,32 @@
       <c r="D11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F11" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="4"/>
+      <c r="H11" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="I11" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J11" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L11" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K11" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L11" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="M11" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N11" s="18">
         <v>512</v>
@@ -1594,15 +1643,15 @@
         <v>9</v>
       </c>
       <c r="W11" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>18</v>
@@ -1610,28 +1659,32 @@
       <c r="D12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F12" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="4"/>
+      <c r="H12" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I12" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J12" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L12" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K12" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L12" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="M12" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N12" s="18">
         <v>512</v>
@@ -1653,15 +1706,15 @@
         <v>9</v>
       </c>
       <c r="W12" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>32</v>
@@ -1669,24 +1722,28 @@
       <c r="D13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F13" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="4"/>
+      <c r="H13" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I13" s="6"/>
       <c r="J13" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L13" s="6"/>
       <c r="M13" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N13" s="4"/>
       <c r="O13" s="6"/>
@@ -1699,12 +1756,12 @@
       <c r="V13" s="4"/>
       <c r="W13" s="6"/>
     </row>
-    <row r="14" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>41</v>
@@ -1712,24 +1769,28 @@
       <c r="D14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F14" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="4"/>
+      <c r="H14" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I14" s="6"/>
       <c r="J14" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L14" s="6"/>
       <c r="M14" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N14" s="4"/>
       <c r="O14" s="6"/>
@@ -1742,12 +1803,12 @@
       <c r="V14" s="4"/>
       <c r="W14" s="6"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>20</v>
@@ -1755,34 +1816,38 @@
       <c r="D15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="4"/>
+      <c r="E15" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F15" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H15" s="4"/>
+      <c r="H15" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="I15" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J15" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L15" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K15" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L15" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="M15" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="N15" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="N15" s="13" t="s">
-        <v>114</v>
-      </c>
       <c r="O15" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P15" s="6" t="s">
         <v>9</v>
@@ -1802,15 +1867,15 @@
         <v>9</v>
       </c>
       <c r="W15" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>21</v>
@@ -1818,34 +1883,38 @@
       <c r="D16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="4"/>
+      <c r="E16" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F16" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H16" s="4"/>
+      <c r="H16" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="I16" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J16" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L16" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K16" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L16" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="M16" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="N16" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="N16" s="17" t="s">
-        <v>114</v>
-      </c>
       <c r="O16" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P16" s="6" t="s">
         <v>9</v>
@@ -1865,40 +1934,44 @@
         <v>9</v>
       </c>
       <c r="W16" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>44</v>
+        <v>129</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="4"/>
+      <c r="E17" s="4" t="s">
+        <v>127</v>
+      </c>
       <c r="F17" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H17" s="4"/>
+      <c r="H17" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I17" s="6"/>
       <c r="J17" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L17" s="6"/>
       <c r="M17" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N17" s="4"/>
       <c r="O17" s="6"/>
@@ -1911,12 +1984,12 @@
       <c r="V17" s="4"/>
       <c r="W17" s="6"/>
     </row>
-    <row r="18" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>19</v>
@@ -1924,24 +1997,28 @@
       <c r="D18" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="4"/>
+      <c r="E18" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F18" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H18" s="4"/>
+      <c r="H18" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I18" s="6"/>
       <c r="J18" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L18" s="6"/>
       <c r="M18" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N18" s="4"/>
       <c r="O18" s="6"/>
@@ -1954,12 +2031,12 @@
       <c r="V18" s="4"/>
       <c r="W18" s="6"/>
     </row>
-    <row r="19" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>42</v>
@@ -1967,24 +2044,28 @@
       <c r="D19" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="4"/>
+      <c r="E19" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F19" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H19" s="4"/>
+      <c r="H19" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I19" s="6"/>
       <c r="J19" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L19" s="6"/>
       <c r="M19" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N19" s="4"/>
       <c r="O19" s="6"/>
@@ -1997,12 +2078,12 @@
       <c r="V19" s="4"/>
       <c r="W19" s="6"/>
     </row>
-    <row r="20" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>40</v>
@@ -2010,24 +2091,28 @@
       <c r="D20" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="4"/>
+      <c r="E20" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F20" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G20" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H20" s="4"/>
+      <c r="H20" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I20" s="6"/>
       <c r="J20" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L20" s="6"/>
       <c r="M20" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N20" s="4"/>
       <c r="O20" s="6"/>
@@ -2040,37 +2125,41 @@
       <c r="V20" s="4"/>
       <c r="W20" s="6"/>
     </row>
-    <row r="21" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="4"/>
+      <c r="E21" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F21" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H21" s="4"/>
+      <c r="H21" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I21" s="6"/>
       <c r="J21" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L21" s="6"/>
       <c r="M21" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N21" s="4"/>
       <c r="O21" s="6"/>
@@ -2083,12 +2172,12 @@
       <c r="V21" s="4"/>
       <c r="W21" s="6"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>22</v>
@@ -2096,28 +2185,32 @@
       <c r="D22" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="4"/>
+      <c r="E22" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F22" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H22" s="4"/>
+      <c r="H22" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="I22" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J22" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L22" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K22" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L22" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="M22" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N22" s="18">
         <v>512</v>
@@ -2139,15 +2232,15 @@
         <v>9</v>
       </c>
       <c r="W22" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>23</v>
@@ -2155,28 +2248,32 @@
       <c r="D23" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="4"/>
+      <c r="E23" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F23" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H23" s="4"/>
+      <c r="H23" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I23" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J23" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L23" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K23" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L23" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="M23" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N23" s="18">
         <v>768</v>
@@ -2195,18 +2292,18 @@
         <v>9</v>
       </c>
       <c r="V23" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="W23" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C24" s="19" t="s">
         <v>24</v>
@@ -2214,28 +2311,32 @@
       <c r="D24" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="4"/>
+      <c r="E24" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F24" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H24" s="4"/>
+      <c r="H24" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I24" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J24" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L24" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K24" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L24" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="M24" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N24" s="22">
         <v>330</v>
@@ -2254,18 +2355,18 @@
         <v>9</v>
       </c>
       <c r="V24" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="W24" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>29</v>
@@ -2273,24 +2374,28 @@
       <c r="D25" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="4"/>
+      <c r="E25" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F25" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H25" s="4"/>
+      <c r="H25" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I25" s="6"/>
       <c r="J25" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L25" s="6"/>
       <c r="M25" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N25" s="4"/>
       <c r="O25" s="6"/>
@@ -2303,12 +2408,12 @@
       <c r="V25" s="4"/>
       <c r="W25" s="6"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>26</v>
@@ -2316,28 +2421,32 @@
       <c r="D26" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="4"/>
+      <c r="E26" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F26" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G26" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H26" s="4"/>
+      <c r="H26" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I26" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J26" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L26" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K26" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L26" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="M26" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N26" s="18">
         <v>330</v>
@@ -2356,18 +2465,18 @@
         <v>9</v>
       </c>
       <c r="V26" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="W26" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>25</v>
@@ -2375,28 +2484,32 @@
       <c r="D27" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="4"/>
+      <c r="E27" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F27" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H27" s="4"/>
+      <c r="H27" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I27" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J27" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L27" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K27" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L27" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="M27" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N27" s="18">
         <v>330</v>
@@ -2415,18 +2528,18 @@
         <v>9</v>
       </c>
       <c r="V27" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="W27" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>27</v>
@@ -2434,28 +2547,32 @@
       <c r="D28" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E28" s="4"/>
+      <c r="E28" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F28" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H28" s="4"/>
+      <c r="H28" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I28" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J28" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L28" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K28" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L28" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="M28" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N28" s="18">
         <v>330</v>
@@ -2474,18 +2591,18 @@
         <v>9</v>
       </c>
       <c r="V28" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="W28" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>28</v>
@@ -2493,34 +2610,38 @@
       <c r="D29" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="4"/>
+      <c r="E29" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F29" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G29" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H29" s="4"/>
+      <c r="H29" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I29" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J29" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L29" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K29" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L29" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="M29" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="N29" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="N29" s="21" t="s">
-        <v>114</v>
-      </c>
       <c r="O29" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P29" s="6" t="s">
         <v>9</v>
@@ -2540,15 +2661,15 @@
         <v>9</v>
       </c>
       <c r="W29" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>30</v>
@@ -2556,34 +2677,38 @@
       <c r="D30" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E30" s="4"/>
+      <c r="E30" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F30" s="6" t="s">
         <v>9</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H30" s="4"/>
+      <c r="H30" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="I30" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J30" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L30" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K30" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L30" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="M30" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="N30" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="N30" s="21" t="s">
-        <v>114</v>
-      </c>
       <c r="O30" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P30" s="6" t="s">
         <v>9</v>
@@ -2603,15 +2728,15 @@
         <v>9</v>
       </c>
       <c r="W30" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>5</v>
@@ -2619,34 +2744,38 @@
       <c r="D31" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E31" s="4"/>
+      <c r="E31" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F31" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H31" s="4"/>
+      <c r="H31" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="I31" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L31" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M31" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="N31" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="N31" s="13" t="s">
-        <v>114</v>
-      </c>
       <c r="O31" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P31" s="6"/>
       <c r="Q31" s="6"/>
@@ -2661,41 +2790,45 @@
         <v>9</v>
       </c>
       <c r="V31" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W31" s="16"/>
     </row>
-    <row r="32" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E32" s="4"/>
+      <c r="E32" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F32" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H32" s="4"/>
+      <c r="H32" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I32" s="6"/>
       <c r="J32" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L32" s="6"/>
       <c r="M32" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N32" s="4"/>
       <c r="O32" s="6"/>
@@ -2708,12 +2841,12 @@
       <c r="V32" s="4"/>
       <c r="W32" s="6"/>
     </row>
-    <row r="33" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>10</v>
@@ -2721,24 +2854,28 @@
       <c r="D33" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E33" s="4"/>
+      <c r="E33" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F33" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G33" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H33" s="4"/>
+      <c r="H33" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I33" s="6"/>
       <c r="J33" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L33" s="6"/>
       <c r="M33" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N33" s="4"/>
       <c r="O33" s="6"/>
@@ -2751,12 +2888,12 @@
       <c r="V33" s="4"/>
       <c r="W33" s="6"/>
     </row>
-    <row r="34" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>12</v>
@@ -2764,24 +2901,28 @@
       <c r="D34" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E34" s="4"/>
+      <c r="E34" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F34" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G34" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H34" s="4"/>
+      <c r="H34" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I34" s="6"/>
       <c r="J34" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L34" s="6"/>
       <c r="M34" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N34" s="4"/>
       <c r="O34" s="6"/>
@@ -2794,37 +2935,41 @@
       <c r="V34" s="4"/>
       <c r="W34" s="6"/>
     </row>
-    <row r="35" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E35" s="4"/>
+      <c r="E35" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F35" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G35" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H35" s="4"/>
+      <c r="H35" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I35" s="6"/>
       <c r="J35" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L35" s="6"/>
       <c r="M35" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N35" s="4"/>
       <c r="O35" s="6"/>
@@ -2837,37 +2982,41 @@
       <c r="V35" s="4"/>
       <c r="W35" s="6"/>
     </row>
-    <row r="36" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E36" s="4"/>
+      <c r="E36" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F36" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H36" s="4"/>
+      <c r="H36" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I36" s="6"/>
       <c r="J36" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K36" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L36" s="6"/>
       <c r="M36" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N36" s="4"/>
       <c r="O36" s="6"/>
@@ -2880,37 +3029,41 @@
       <c r="V36" s="4"/>
       <c r="W36" s="6"/>
     </row>
-    <row r="37" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E37" s="4"/>
+      <c r="E37" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F37" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H37" s="4"/>
+      <c r="H37" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I37" s="6"/>
       <c r="J37" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L37" s="6"/>
       <c r="M37" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N37" s="4"/>
       <c r="O37" s="6"/>
@@ -2923,12 +3076,12 @@
       <c r="V37" s="4"/>
       <c r="W37" s="6"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>6</v>
@@ -2936,34 +3089,38 @@
       <c r="D38" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E38" s="4"/>
+      <c r="E38" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F38" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G38" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H38" s="4"/>
+      <c r="H38" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="I38" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K38" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L38" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M38" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="N38" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="N38" s="13" t="s">
-        <v>114</v>
-      </c>
       <c r="O38" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P38" s="6"/>
       <c r="Q38" s="6"/>
@@ -2980,12 +3137,12 @@
       <c r="V38" s="4"/>
       <c r="W38" s="16"/>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>37</v>
@@ -2993,34 +3150,38 @@
       <c r="D39" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E39" s="4"/>
+      <c r="E39" s="4" t="s">
+        <v>127</v>
+      </c>
       <c r="F39" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G39" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H39" s="4"/>
+      <c r="H39" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="I39" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J39" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L39" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K39" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L39" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="M39" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="N39" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="N39" s="21" t="s">
-        <v>114</v>
-      </c>
       <c r="O39" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P39" s="6" t="s">
         <v>9</v>
@@ -3040,44 +3201,48 @@
         <v>9</v>
       </c>
       <c r="W39" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E40" s="4"/>
+      <c r="E40" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F40" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H40" s="4"/>
+      <c r="H40" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I40" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J40" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K40" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L40" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K40" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L40" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="M40" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N40" s="18">
         <v>330</v>
@@ -3096,47 +3261,51 @@
         <v>9</v>
       </c>
       <c r="V40" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="W40" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E41" s="4"/>
+      <c r="E41" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F41" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H41" s="4"/>
+      <c r="H41" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I41" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J41" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K41" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L41" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K41" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L41" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="M41" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N41" s="18">
         <v>330</v>
@@ -3155,47 +3324,51 @@
         <v>9</v>
       </c>
       <c r="V41" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="W41" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E42" s="4"/>
+      <c r="E42" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F42" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H42" s="4"/>
+      <c r="H42" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I42" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J42" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K42" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L42" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K42" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L42" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="M42" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N42" s="18">
         <v>330</v>
@@ -3214,47 +3387,51 @@
         <v>9</v>
       </c>
       <c r="V42" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="W42" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E43" s="4"/>
+      <c r="E43" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F43" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G43" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H43" s="4"/>
+      <c r="H43" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I43" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J43" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K43" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L43" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K43" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L43" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="M43" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N43" s="22">
         <v>1200</v>
@@ -3273,53 +3450,57 @@
         <v>9</v>
       </c>
       <c r="V43" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="W43" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E44" s="4"/>
+      <c r="E44" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F44" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G44" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H44" s="4"/>
+      <c r="H44" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I44" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J44" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K44" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L44" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K44" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L44" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="M44" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="N44" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="N44" s="13" t="s">
-        <v>114</v>
-      </c>
       <c r="O44" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P44" s="6" t="s">
         <v>9</v>
@@ -3339,44 +3520,48 @@
         <v>9</v>
       </c>
       <c r="W44" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E45" s="4"/>
+      <c r="E45" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F45" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G45" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H45" s="4"/>
+      <c r="H45" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I45" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J45" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K45" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L45" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K45" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L45" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="M45" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N45" s="18">
         <v>1200</v>
@@ -3395,47 +3580,51 @@
         <v>9</v>
       </c>
       <c r="V45" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="W45" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E46" s="4"/>
+      <c r="E46" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F46" s="6" t="s">
         <v>9</v>
       </c>
       <c r="G46" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H46" s="4"/>
+      <c r="H46" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I46" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J46" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K46" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L46" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K46" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L46" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="M46" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N46" s="18">
         <v>1200</v>
@@ -3454,47 +3643,51 @@
         <v>9</v>
       </c>
       <c r="V46" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="W46" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E47" s="4"/>
+      <c r="E47" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F47" s="6" t="s">
         <v>9</v>
       </c>
       <c r="G47" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H47" s="4"/>
+      <c r="H47" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="I47" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J47" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K47" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L47" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K47" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L47" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="M47" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N47" s="18">
         <v>1200</v>
@@ -3513,47 +3706,51 @@
         <v>9</v>
       </c>
       <c r="V47" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="W47" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E48" s="4"/>
+      <c r="E48" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F48" s="6" t="s">
         <v>9</v>
       </c>
       <c r="G48" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H48" s="4"/>
+      <c r="H48" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I48" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J48" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K48" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L48" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K48" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L48" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="M48" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N48" s="22">
         <v>128</v>
@@ -3572,53 +3769,57 @@
         <v>9</v>
       </c>
       <c r="V48" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="W48" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E49" s="4"/>
+      <c r="E49" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F49" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G49" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H49" s="4"/>
+      <c r="H49" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I49" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J49" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K49" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L49" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K49" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L49" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="M49" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="N49" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="N49" s="23" t="s">
-        <v>114</v>
-      </c>
       <c r="O49" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P49" s="6" t="s">
         <v>9</v>
@@ -3638,15 +3839,15 @@
         <v>9</v>
       </c>
       <c r="W49" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="50" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>35</v>
@@ -3654,24 +3855,28 @@
       <c r="D50" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E50" s="4"/>
+      <c r="E50" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F50" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G50" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H50" s="4"/>
+      <c r="H50" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I50" s="6"/>
       <c r="J50" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K50" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L50" s="6"/>
       <c r="M50" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N50" s="4"/>
       <c r="O50" s="6"/>
@@ -3684,12 +3889,12 @@
       <c r="V50" s="4"/>
       <c r="W50" s="6"/>
     </row>
-    <row r="51" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>38</v>
@@ -3697,24 +3902,28 @@
       <c r="D51" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E51" s="4"/>
+      <c r="E51" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F51" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G51" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H51" s="4"/>
+      <c r="H51" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I51" s="6"/>
       <c r="J51" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K51" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L51" s="6"/>
       <c r="M51" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N51" s="4"/>
       <c r="O51" s="6"/>
@@ -3727,41 +3936,45 @@
       <c r="V51" s="4"/>
       <c r="W51" s="6"/>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E52" s="4"/>
+      <c r="E52" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F52" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G52" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H52" s="4"/>
+      <c r="H52" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I52" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J52" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K52" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L52" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K52" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L52" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="M52" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N52" s="18">
         <v>512</v>
@@ -3783,44 +3996,48 @@
         <v>9</v>
       </c>
       <c r="W52" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E53" s="4"/>
+      <c r="E53" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F53" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G53" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H53" s="4"/>
+      <c r="H53" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I53" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J53" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K53" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L53" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K53" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L53" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="M53" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N53" s="18">
         <v>330</v>
@@ -3839,18 +4056,18 @@
         <v>9</v>
       </c>
       <c r="V53" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="W53" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="54" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>4</v>
@@ -3858,24 +4075,28 @@
       <c r="D54" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E54" s="4"/>
+      <c r="E54" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F54" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G54" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H54" s="4"/>
+      <c r="H54" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I54" s="6"/>
       <c r="J54" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K54" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L54" s="6"/>
       <c r="M54" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N54" s="4"/>
       <c r="O54" s="6"/>
@@ -3888,12 +4109,12 @@
       <c r="V54" s="4"/>
       <c r="W54" s="6"/>
     </row>
-    <row r="55" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>33</v>
@@ -3901,24 +4122,28 @@
       <c r="D55" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E55" s="4"/>
+      <c r="E55" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F55" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G55" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H55" s="4"/>
+      <c r="H55" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I55" s="6"/>
       <c r="J55" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K55" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L55" s="6"/>
       <c r="M55" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N55" s="4"/>
       <c r="O55" s="6"/>
@@ -3931,37 +4156,41 @@
       <c r="V55" s="4"/>
       <c r="W55" s="6"/>
     </row>
-    <row r="56" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E56" s="4"/>
+      <c r="E56" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F56" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G56" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H56" s="4"/>
+      <c r="H56" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I56" s="6"/>
       <c r="J56" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K56" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L56" s="6"/>
       <c r="M56" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N56" s="4"/>
       <c r="O56" s="6"/>
@@ -3974,41 +4203,45 @@
       <c r="V56" s="4"/>
       <c r="W56" s="6"/>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E57" s="4"/>
+      <c r="E57" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F57" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G57" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H57" s="4"/>
+      <c r="H57" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I57" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J57" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K57" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L57" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K57" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L57" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="M57" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N57" s="18">
         <v>512</v>
@@ -4030,50 +4263,54 @@
         <v>9</v>
       </c>
       <c r="W57" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E58" s="4"/>
+      <c r="E58" s="4" t="s">
+        <v>127</v>
+      </c>
       <c r="F58" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G58" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H58" s="4"/>
+      <c r="H58" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="I58" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J58" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K58" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L58" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K58" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L58" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="M58" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="N58" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="N58" s="21" t="s">
-        <v>114</v>
-      </c>
       <c r="O58" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P58" s="6" t="s">
         <v>9</v>
@@ -4093,15 +4330,15 @@
         <v>9</v>
       </c>
       <c r="W58" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="59" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C59" s="7" t="s">
         <v>34</v>
@@ -4109,24 +4346,28 @@
       <c r="D59" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E59" s="4"/>
+      <c r="E59" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F59" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G59" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H59" s="4"/>
+      <c r="H59" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I59" s="6"/>
       <c r="J59" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K59" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L59" s="6"/>
       <c r="M59" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N59" s="4"/>
       <c r="O59" s="6"/>
@@ -4139,12 +4380,12 @@
       <c r="V59" s="4"/>
       <c r="W59" s="6"/>
     </row>
-    <row r="60" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>36</v>
@@ -4152,24 +4393,28 @@
       <c r="D60" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E60" s="4"/>
+      <c r="E60" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F60" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G60" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H60" s="4"/>
+      <c r="H60" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I60" s="6"/>
       <c r="J60" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K60" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L60" s="6"/>
       <c r="M60" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N60" s="4"/>
       <c r="O60" s="6"/>
@@ -4182,12 +4427,12 @@
       <c r="V60" s="4"/>
       <c r="W60" s="6"/>
     </row>
-    <row r="61" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C61" s="10" t="s">
         <v>1</v>
@@ -4195,24 +4440,28 @@
       <c r="D61" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E61" s="4"/>
+      <c r="E61" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F61" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G61" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H61" s="4"/>
+      <c r="H61" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I61" s="6"/>
       <c r="J61" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K61" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L61" s="6"/>
       <c r="M61" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N61" s="4"/>
       <c r="O61" s="6"/>
@@ -4225,12 +4474,12 @@
       <c r="V61" s="4"/>
       <c r="W61" s="6"/>
     </row>
-    <row r="62" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>7</v>
@@ -4238,24 +4487,28 @@
       <c r="D62" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E62" s="4"/>
+      <c r="E62" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F62" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G62" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H62" s="4"/>
+      <c r="H62" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I62" s="6"/>
       <c r="J62" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K62" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L62" s="6"/>
       <c r="M62" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N62" s="4"/>
       <c r="O62" s="6"/>
@@ -4268,12 +4521,12 @@
       <c r="V62" s="4"/>
       <c r="W62" s="6"/>
     </row>
-    <row r="63" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>43</v>
@@ -4281,24 +4534,28 @@
       <c r="D63" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E63" s="4"/>
+      <c r="E63" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F63" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G63" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H63" s="4"/>
+      <c r="H63" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I63" s="6"/>
       <c r="J63" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K63" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L63" s="6"/>
       <c r="M63" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N63" s="4"/>
       <c r="O63" s="6"/>
@@ -4311,12 +4568,12 @@
       <c r="V63" s="4"/>
       <c r="W63" s="6"/>
     </row>
-    <row r="64" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>13</v>
@@ -4324,24 +4581,28 @@
       <c r="D64" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E64" s="4"/>
+      <c r="E64" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F64" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G64" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H64" s="4"/>
+      <c r="H64" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I64" s="6"/>
       <c r="J64" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K64" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L64" s="6"/>
       <c r="M64" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N64" s="4"/>
       <c r="O64" s="6"/>
@@ -4354,37 +4615,41 @@
       <c r="V64" s="4"/>
       <c r="W64" s="6"/>
     </row>
-    <row r="65" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E65" s="4"/>
+      <c r="E65" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F65" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G65" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H65" s="4"/>
+      <c r="H65" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="I65" s="6"/>
       <c r="J65" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K65" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L65" s="6"/>
       <c r="M65" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N65" s="4"/>
       <c r="O65" s="6"/>
@@ -4399,9 +4664,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[MDTUDDM-28147] Registry services requirements.
Change-Id: I7d4f5bc2caf4814576f190f495eb4a0f0b761cb3
</commit_message>
<xml_diff>
--- a/docs/ua/modules/arch/attachments/architecture-workspace/registry-resources.xlsx
+++ b/docs/ua/modules/arch/attachments/architecture-workspace/registry-resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruslan_Lesyk\Desktop\ddm-architecture\docs\ua\modules\arch\attachments\architecture-workspace\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Maksym_Kharchenko/Work/Development/mdtu-ddm/mdtu-ddm-gerrit-workspace/mdtu-ddm/general/ddm-architecture/docs/ua/modules/arch/attachments/architecture-workspace/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7866B66D-60E5-4490-8292-4F0DBCCBB5CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA63AE4F-486F-6A43-9D82-D1A888F87420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{76BACE1B-BDCC-F34F-9205-7BB42BE8027F}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="23260" windowHeight="12460" xr2:uid="{76BACE1B-BDCC-F34F-9205-7BB42BE8027F}"/>
   </bookViews>
   <sheets>
     <sheet name="Registry Resources" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="129">
   <si>
     <t>Technology</t>
   </si>
@@ -378,9 +378,6 @@
   </si>
   <si>
     <t>?</t>
-  </si>
-  <si>
-    <t>-XX:+UseG1GC -XX:+ExplicitGCInvokesConcurrent -Duser.timezone=UTC</t>
   </si>
   <si>
     <t>-Xms=256M -XX:+ExplicitGCInvokesConcurrent -XX:G1HeapRegionSize=16M -XX:InitiatingHeapOccupancyPercent=35 -XX:MaxGCPauseMillis=20 -XX:MaxMetaspaceFreeRatio=80 -XX:MetaspaceSize=96m -XX:MinMetaspaceFreeRatio=50 -XX:+UseG1GC</t>
@@ -1042,38 +1039,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C809D083-7CF6-1445-A306-E810BD791428}">
   <dimension ref="A1:W65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W31" sqref="W31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.796875" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="65.796875" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="65.83203125" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="35.5" customWidth="1"/>
     <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="21.09765625" customWidth="1"/>
-    <col min="6" max="6" width="14.296875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="2" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="2" customWidth="1"/>
     <col min="8" max="8" width="15.5" customWidth="1"/>
-    <col min="9" max="9" width="14.296875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="18.796875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.69921875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="18.83203125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" style="2" customWidth="1"/>
     <col min="12" max="12" width="21" style="2" customWidth="1"/>
-    <col min="13" max="13" width="21.296875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="21.33203125" style="2" customWidth="1"/>
     <col min="14" max="14" width="21.5" customWidth="1"/>
-    <col min="15" max="15" width="19.796875" customWidth="1"/>
+    <col min="15" max="15" width="19.83203125" customWidth="1"/>
     <col min="16" max="16" width="20.5" customWidth="1"/>
-    <col min="17" max="17" width="26.296875" customWidth="1"/>
+    <col min="17" max="17" width="26.33203125" customWidth="1"/>
     <col min="18" max="18" width="15.5" customWidth="1"/>
     <col min="19" max="19" width="19.5" customWidth="1"/>
-    <col min="20" max="20" width="18.19921875" customWidth="1"/>
+    <col min="20" max="20" width="18.1640625" customWidth="1"/>
     <col min="21" max="21" width="18.5" customWidth="1"/>
-    <col min="22" max="22" width="65.69921875" customWidth="1"/>
-    <col min="23" max="23" width="66.69921875" style="3" customWidth="1"/>
+    <col min="22" max="22" width="65.6640625" customWidth="1"/>
+    <col min="23" max="23" width="66.6640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>95</v>
       </c>
@@ -1114,37 +1111,37 @@
         <v>108</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="V1" t="s">
+        <v>115</v>
+      </c>
+      <c r="W1" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="W1" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" ht="16.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:23" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>72</v>
       </c>
@@ -1158,7 +1155,7 @@
         <v>15</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>3</v>
@@ -1191,7 +1188,7 @@
       <c r="V2" s="4"/>
       <c r="W2" s="6"/>
     </row>
-    <row r="3" spans="1:23" ht="16.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>72</v>
       </c>
@@ -1205,7 +1202,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>3</v>
@@ -1238,7 +1235,7 @@
       <c r="V3" s="4"/>
       <c r="W3" s="6"/>
     </row>
-    <row r="4" spans="1:23" ht="16.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>72</v>
       </c>
@@ -1252,7 +1249,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>3</v>
@@ -1285,7 +1282,7 @@
       <c r="V4" s="4"/>
       <c r="W4" s="6"/>
     </row>
-    <row r="5" spans="1:23" ht="16.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>72</v>
       </c>
@@ -1299,7 +1296,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>3</v>
@@ -1332,7 +1329,7 @@
       <c r="V5" s="4"/>
       <c r="W5" s="6"/>
     </row>
-    <row r="6" spans="1:23" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>73</v>
       </c>
@@ -1346,7 +1343,7 @@
         <v>15</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>3</v>
@@ -1355,7 +1352,7 @@
         <v>3</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>91</v>
@@ -1391,11 +1388,9 @@
       <c r="V6" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="W6" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" ht="16.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W6" s="16"/>
+    </row>
+    <row r="7" spans="1:23" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>72</v>
       </c>
@@ -1409,7 +1404,7 @@
         <v>15</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>3</v>
@@ -1442,7 +1437,7 @@
       <c r="V7" s="4"/>
       <c r="W7" s="6"/>
     </row>
-    <row r="8" spans="1:23" ht="16.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>72</v>
       </c>
@@ -1456,7 +1451,7 @@
         <v>15</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>3</v>
@@ -1489,7 +1484,7 @@
       <c r="V8" s="4"/>
       <c r="W8" s="6"/>
     </row>
-    <row r="9" spans="1:23" ht="16.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>72</v>
       </c>
@@ -1503,7 +1498,7 @@
         <v>15</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>3</v>
@@ -1536,7 +1531,7 @@
       <c r="V9" s="4"/>
       <c r="W9" s="6"/>
     </row>
-    <row r="10" spans="1:23" ht="16.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>72</v>
       </c>
@@ -1550,7 +1545,7 @@
         <v>15</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>3</v>
@@ -1583,7 +1578,7 @@
       <c r="V10" s="4"/>
       <c r="W10" s="6"/>
     </row>
-    <row r="11" spans="1:23" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>73</v>
       </c>
@@ -1597,7 +1592,7 @@
         <v>15</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>3</v>
@@ -1642,11 +1637,9 @@
       <c r="V11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="W11" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W11" s="16"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>72</v>
       </c>
@@ -1660,7 +1653,7 @@
         <v>15</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>3</v>
@@ -1705,11 +1698,9 @@
       <c r="V12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="W12" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+      <c r="W12" s="16"/>
+    </row>
+    <row r="13" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>72</v>
       </c>
@@ -1723,7 +1714,7 @@
         <v>15</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>3</v>
@@ -1756,7 +1747,7 @@
       <c r="V13" s="4"/>
       <c r="W13" s="6"/>
     </row>
-    <row r="14" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>72</v>
       </c>
@@ -1770,7 +1761,7 @@
         <v>15</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>3</v>
@@ -1803,7 +1794,7 @@
       <c r="V14" s="4"/>
       <c r="W14" s="6"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>72</v>
       </c>
@@ -1817,7 +1808,7 @@
         <v>15</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>3</v>
@@ -1866,11 +1857,9 @@
       <c r="V15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="W15" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W15" s="16"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>73</v>
       </c>
@@ -1884,7 +1873,7 @@
         <v>15</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>3</v>
@@ -1933,11 +1922,9 @@
       <c r="V16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="W16" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+      <c r="W16" s="16"/>
+    </row>
+    <row r="17" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>72</v>
       </c>
@@ -1945,13 +1932,13 @@
         <v>71</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>3</v>
@@ -1984,7 +1971,7 @@
       <c r="V17" s="4"/>
       <c r="W17" s="6"/>
     </row>
-    <row r="18" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>73</v>
       </c>
@@ -1998,7 +1985,7 @@
         <v>15</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>3</v>
@@ -2031,7 +2018,7 @@
       <c r="V18" s="4"/>
       <c r="W18" s="6"/>
     </row>
-    <row r="19" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>73</v>
       </c>
@@ -2045,7 +2032,7 @@
         <v>15</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>3</v>
@@ -2078,7 +2065,7 @@
       <c r="V19" s="4"/>
       <c r="W19" s="6"/>
     </row>
-    <row r="20" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>73</v>
       </c>
@@ -2092,7 +2079,7 @@
         <v>15</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>3</v>
@@ -2125,7 +2112,7 @@
       <c r="V20" s="4"/>
       <c r="W20" s="6"/>
     </row>
-    <row r="21" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>73</v>
       </c>
@@ -2139,7 +2126,7 @@
         <v>15</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>3</v>
@@ -2172,7 +2159,7 @@
       <c r="V21" s="4"/>
       <c r="W21" s="6"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>73</v>
       </c>
@@ -2186,7 +2173,7 @@
         <v>15</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>3</v>
@@ -2231,11 +2218,9 @@
       <c r="V22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="W22" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W22" s="16"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>73</v>
       </c>
@@ -2249,7 +2234,7 @@
         <v>15</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>3</v>
@@ -2294,11 +2279,9 @@
       <c r="V23" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="W23" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W23" s="16"/>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>73</v>
       </c>
@@ -2312,7 +2295,7 @@
         <v>15</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>3</v>
@@ -2357,11 +2340,9 @@
       <c r="V24" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="W24" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W24" s="16"/>
+    </row>
+    <row r="25" spans="1:23" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>73</v>
       </c>
@@ -2375,7 +2356,7 @@
         <v>15</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>3</v>
@@ -2408,7 +2389,7 @@
       <c r="V25" s="4"/>
       <c r="W25" s="6"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>73</v>
       </c>
@@ -2422,7 +2403,7 @@
         <v>15</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>3</v>
@@ -2467,11 +2448,9 @@
       <c r="V26" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="W26" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W26" s="16"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>73</v>
       </c>
@@ -2485,7 +2464,7 @@
         <v>15</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>3</v>
@@ -2530,11 +2509,9 @@
       <c r="V27" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="W27" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W27" s="16"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>73</v>
       </c>
@@ -2548,7 +2525,7 @@
         <v>15</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>3</v>
@@ -2593,11 +2570,9 @@
       <c r="V28" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="W28" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W28" s="16"/>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>73</v>
       </c>
@@ -2611,7 +2586,7 @@
         <v>15</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>3</v>
@@ -2660,11 +2635,9 @@
       <c r="V29" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="W29" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W29" s="16"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>73</v>
       </c>
@@ -2678,7 +2651,7 @@
         <v>15</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>9</v>
@@ -2727,11 +2700,9 @@
       <c r="V30" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="W30" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="W30" s="16"/>
+    </row>
+    <row r="31" spans="1:23" ht="68" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>73</v>
       </c>
@@ -2745,7 +2716,7 @@
         <v>2</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>3</v>
@@ -2790,11 +2761,11 @@
         <v>9</v>
       </c>
       <c r="V31" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="W31" s="16"/>
     </row>
-    <row r="32" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>73</v>
       </c>
@@ -2808,7 +2779,7 @@
         <v>15</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>3</v>
@@ -2841,7 +2812,7 @@
       <c r="V32" s="4"/>
       <c r="W32" s="6"/>
     </row>
-    <row r="33" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>73</v>
       </c>
@@ -2855,7 +2826,7 @@
         <v>2</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>3</v>
@@ -2888,7 +2859,7 @@
       <c r="V33" s="4"/>
       <c r="W33" s="6"/>
     </row>
-    <row r="34" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>73</v>
       </c>
@@ -2902,7 +2873,7 @@
         <v>2</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>3</v>
@@ -2935,7 +2906,7 @@
       <c r="V34" s="4"/>
       <c r="W34" s="6"/>
     </row>
-    <row r="35" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>73</v>
       </c>
@@ -2949,7 +2920,7 @@
         <v>15</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>3</v>
@@ -2982,7 +2953,7 @@
       <c r="V35" s="4"/>
       <c r="W35" s="6"/>
     </row>
-    <row r="36" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>73</v>
       </c>
@@ -2996,7 +2967,7 @@
         <v>15</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>3</v>
@@ -3029,7 +3000,7 @@
       <c r="V36" s="4"/>
       <c r="W36" s="6"/>
     </row>
-    <row r="37" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>73</v>
       </c>
@@ -3043,7 +3014,7 @@
         <v>15</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>3</v>
@@ -3076,7 +3047,7 @@
       <c r="V37" s="4"/>
       <c r="W37" s="6"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>73</v>
       </c>
@@ -3090,7 +3061,7 @@
         <v>2</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>3</v>
@@ -3137,7 +3108,7 @@
       <c r="V38" s="4"/>
       <c r="W38" s="16"/>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>72</v>
       </c>
@@ -3151,7 +3122,7 @@
         <v>15</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>3</v>
@@ -3200,11 +3171,9 @@
       <c r="V39" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="W39" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W39" s="16"/>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>73</v>
       </c>
@@ -3218,7 +3187,7 @@
         <v>15</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>3</v>
@@ -3263,11 +3232,9 @@
       <c r="V40" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="W40" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W40" s="16"/>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>73</v>
       </c>
@@ -3281,7 +3248,7 @@
         <v>15</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>3</v>
@@ -3326,11 +3293,9 @@
       <c r="V41" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="W41" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W41" s="16"/>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>73</v>
       </c>
@@ -3344,7 +3309,7 @@
         <v>15</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F42" s="6" t="s">
         <v>3</v>
@@ -3389,11 +3354,9 @@
       <c r="V42" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="W42" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W42" s="16"/>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>73</v>
       </c>
@@ -3407,7 +3370,7 @@
         <v>15</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>3</v>
@@ -3452,11 +3415,9 @@
       <c r="V43" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="W43" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W43" s="16"/>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>72</v>
       </c>
@@ -3470,7 +3431,7 @@
         <v>15</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>3</v>
@@ -3519,11 +3480,9 @@
       <c r="V44" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="W44" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W44" s="16"/>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>73</v>
       </c>
@@ -3537,7 +3496,7 @@
         <v>15</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F45" s="6" t="s">
         <v>3</v>
@@ -3582,11 +3541,9 @@
       <c r="V45" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="W45" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W45" s="16"/>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>73</v>
       </c>
@@ -3600,7 +3557,7 @@
         <v>15</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F46" s="6" t="s">
         <v>9</v>
@@ -3645,11 +3602,9 @@
       <c r="V46" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="W46" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W46" s="16"/>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>73</v>
       </c>
@@ -3663,7 +3618,7 @@
         <v>15</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>9</v>
@@ -3708,11 +3663,9 @@
       <c r="V47" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="W47" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W47" s="16"/>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>73</v>
       </c>
@@ -3726,7 +3679,7 @@
         <v>15</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>9</v>
@@ -3771,11 +3724,9 @@
       <c r="V48" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="W48" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W48" s="16"/>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>72</v>
       </c>
@@ -3789,7 +3740,7 @@
         <v>15</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>3</v>
@@ -3838,11 +3789,9 @@
       <c r="V49" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="W49" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="50" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+      <c r="W49" s="16"/>
+    </row>
+    <row r="50" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>73</v>
       </c>
@@ -3856,7 +3805,7 @@
         <v>15</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>3</v>
@@ -3889,7 +3838,7 @@
       <c r="V50" s="4"/>
       <c r="W50" s="6"/>
     </row>
-    <row r="51" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>73</v>
       </c>
@@ -3903,7 +3852,7 @@
         <v>15</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>3</v>
@@ -3936,7 +3885,7 @@
       <c r="V51" s="4"/>
       <c r="W51" s="6"/>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>73</v>
       </c>
@@ -3950,7 +3899,7 @@
         <v>15</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>3</v>
@@ -3995,11 +3944,9 @@
       <c r="V52" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="W52" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W52" s="16"/>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>73</v>
       </c>
@@ -4013,7 +3960,7 @@
         <v>15</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>3</v>
@@ -4058,11 +4005,9 @@
       <c r="V53" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="W53" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="54" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+      <c r="W53" s="16"/>
+    </row>
+    <row r="54" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>73</v>
       </c>
@@ -4076,7 +4021,7 @@
         <v>2</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>3</v>
@@ -4109,7 +4054,7 @@
       <c r="V54" s="4"/>
       <c r="W54" s="6"/>
     </row>
-    <row r="55" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>73</v>
       </c>
@@ -4123,7 +4068,7 @@
         <v>15</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>3</v>
@@ -4156,7 +4101,7 @@
       <c r="V55" s="4"/>
       <c r="W55" s="6"/>
     </row>
-    <row r="56" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>73</v>
       </c>
@@ -4170,7 +4115,7 @@
         <v>15</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>3</v>
@@ -4203,7 +4148,7 @@
       <c r="V56" s="4"/>
       <c r="W56" s="6"/>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>73</v>
       </c>
@@ -4217,7 +4162,7 @@
         <v>15</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>3</v>
@@ -4262,11 +4207,9 @@
       <c r="V57" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="W57" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W57" s="16"/>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>73</v>
       </c>
@@ -4280,7 +4223,7 @@
         <v>15</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F58" s="6" t="s">
         <v>3</v>
@@ -4329,11 +4272,9 @@
       <c r="V58" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="W58" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="59" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+      <c r="W58" s="16"/>
+    </row>
+    <row r="59" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>73</v>
       </c>
@@ -4347,7 +4288,7 @@
         <v>15</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>3</v>
@@ -4380,7 +4321,7 @@
       <c r="V59" s="4"/>
       <c r="W59" s="6"/>
     </row>
-    <row r="60" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>73</v>
       </c>
@@ -4394,7 +4335,7 @@
         <v>15</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>3</v>
@@ -4427,7 +4368,7 @@
       <c r="V60" s="4"/>
       <c r="W60" s="6"/>
     </row>
-    <row r="61" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>73</v>
       </c>
@@ -4441,7 +4382,7 @@
         <v>2</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F61" s="6" t="s">
         <v>3</v>
@@ -4474,7 +4415,7 @@
       <c r="V61" s="4"/>
       <c r="W61" s="6"/>
     </row>
-    <row r="62" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>73</v>
       </c>
@@ -4488,7 +4429,7 @@
         <v>2</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F62" s="6" t="s">
         <v>3</v>
@@ -4521,7 +4462,7 @@
       <c r="V62" s="4"/>
       <c r="W62" s="6"/>
     </row>
-    <row r="63" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>73</v>
       </c>
@@ -4535,7 +4476,7 @@
         <v>15</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F63" s="6" t="s">
         <v>3</v>
@@ -4568,7 +4509,7 @@
       <c r="V63" s="4"/>
       <c r="W63" s="6"/>
     </row>
-    <row r="64" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>73</v>
       </c>
@@ -4582,7 +4523,7 @@
         <v>2</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F64" s="6" t="s">
         <v>3</v>
@@ -4615,7 +4556,7 @@
       <c r="V64" s="4"/>
       <c r="W64" s="6"/>
     </row>
-    <row r="65" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>73</v>
       </c>
@@ -4629,7 +4570,7 @@
         <v>15</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F65" s="6" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
[MDTUDDM-28611] - Updated current registry resources state
Change-Id: I5d66dc1f7d9f365500c63fa01e17652ff8024a3e
</commit_message>
<xml_diff>
--- a/docs/ua/modules/arch/attachments/architecture-workspace/registry-resources.xlsx
+++ b/docs/ua/modules/arch/attachments/architecture-workspace/registry-resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Maksym_Kharchenko/Work/Development/mdtu-ddm/mdtu-ddm-gerrit-workspace/mdtu-ddm/general/ddm-architecture/docs/ua/modules/arch/attachments/architecture-workspace/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\mdtu-ddm\ddm-architecture\docs\ua\modules\arch\attachments\architecture-workspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA63AE4F-486F-6A43-9D82-D1A888F87420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C158A8-25FC-4510-9E9D-6AD576FA1915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="23260" windowHeight="12460" xr2:uid="{76BACE1B-BDCC-F34F-9205-7BB42BE8027F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{76BACE1B-BDCC-F34F-9205-7BB42BE8027F}"/>
   </bookViews>
   <sheets>
     <sheet name="Registry Resources" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="129">
   <si>
     <t>Technology</t>
   </si>
@@ -701,13 +701,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{06C99DE8-B980-0548-85E0-AAF92621FDD9}" name="Table3" displayName="Table3" ref="A1:W65" totalsRowShown="0" dataDxfId="23">
-  <autoFilter ref="A1:W65" xr:uid="{06C99DE8-B980-0548-85E0-AAF92621FDD9}">
-    <filterColumn colId="8">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:W65" xr:uid="{06C99DE8-B980-0548-85E0-AAF92621FDD9}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:W58">
     <sortCondition ref="C1:C65"/>
   </sortState>
@@ -1039,38 +1033,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C809D083-7CF6-1445-A306-E810BD791428}">
   <dimension ref="A1:W65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W31" sqref="W31"/>
+    <sheetView tabSelected="1" topLeftCell="C23" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L57" sqref="L57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.83203125" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="65.83203125" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="28.796875" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="65.796875" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="35.5" customWidth="1"/>
     <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="21.1640625" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.19921875" customWidth="1"/>
+    <col min="6" max="6" width="14.296875" style="2" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="2" customWidth="1"/>
     <col min="8" max="8" width="15.5" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="18.83203125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="14.296875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="18.796875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.69921875" style="2" customWidth="1"/>
     <col min="12" max="12" width="21" style="2" customWidth="1"/>
-    <col min="13" max="13" width="21.33203125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="21.296875" style="2" customWidth="1"/>
     <col min="14" max="14" width="21.5" customWidth="1"/>
-    <col min="15" max="15" width="19.83203125" customWidth="1"/>
+    <col min="15" max="15" width="19.796875" customWidth="1"/>
     <col min="16" max="16" width="20.5" customWidth="1"/>
-    <col min="17" max="17" width="26.33203125" customWidth="1"/>
+    <col min="17" max="17" width="26.296875" customWidth="1"/>
     <col min="18" max="18" width="15.5" customWidth="1"/>
     <col min="19" max="19" width="19.5" customWidth="1"/>
-    <col min="20" max="20" width="18.1640625" customWidth="1"/>
+    <col min="20" max="20" width="18.19921875" customWidth="1"/>
     <col min="21" max="21" width="18.5" customWidth="1"/>
-    <col min="22" max="22" width="65.6640625" customWidth="1"/>
-    <col min="23" max="23" width="66.6640625" style="3" customWidth="1"/>
+    <col min="22" max="22" width="65.69921875" customWidth="1"/>
+    <col min="23" max="23" width="66.69921875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>95</v>
       </c>
@@ -1141,7 +1135,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>72</v>
       </c>
@@ -1188,7 +1182,7 @@
       <c r="V2" s="4"/>
       <c r="W2" s="6"/>
     </row>
-    <row r="3" spans="1:23" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>72</v>
       </c>
@@ -1235,7 +1229,7 @@
       <c r="V3" s="4"/>
       <c r="W3" s="6"/>
     </row>
-    <row r="4" spans="1:23" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>72</v>
       </c>
@@ -1282,7 +1276,7 @@
       <c r="V4" s="4"/>
       <c r="W4" s="6"/>
     </row>
-    <row r="5" spans="1:23" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>72</v>
       </c>
@@ -1329,7 +1323,7 @@
       <c r="V5" s="4"/>
       <c r="W5" s="6"/>
     </row>
-    <row r="6" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>73</v>
       </c>
@@ -1390,7 +1384,7 @@
       </c>
       <c r="W6" s="16"/>
     </row>
-    <row r="7" spans="1:23" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>72</v>
       </c>
@@ -1413,21 +1407,29 @@
         <v>9</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I7" s="6"/>
+        <v>9</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>91</v>
+      </c>
       <c r="J7" s="6" t="s">
         <v>110</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="L7" s="6"/>
+      <c r="L7" s="11" t="s">
+        <v>113</v>
+      </c>
       <c r="M7" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="N7" s="4"/>
-      <c r="O7" s="6"/>
+      <c r="N7" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="O7" s="13" t="s">
+        <v>113</v>
+      </c>
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
@@ -1437,7 +1439,7 @@
       <c r="V7" s="4"/>
       <c r="W7" s="6"/>
     </row>
-    <row r="8" spans="1:23" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>72</v>
       </c>
@@ -1484,7 +1486,7 @@
       <c r="V8" s="4"/>
       <c r="W8" s="6"/>
     </row>
-    <row r="9" spans="1:23" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>72</v>
       </c>
@@ -1531,7 +1533,7 @@
       <c r="V9" s="4"/>
       <c r="W9" s="6"/>
     </row>
-    <row r="10" spans="1:23" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>72</v>
       </c>
@@ -1578,7 +1580,7 @@
       <c r="V10" s="4"/>
       <c r="W10" s="6"/>
     </row>
-    <row r="11" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>73</v>
       </c>
@@ -1600,8 +1602,9 @@
       <c r="G11" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="6" t="s">
-        <v>9</v>
+      <c r="H11" s="6" t="str">
+        <f>+H6</f>
+        <v xml:space="preserve"> +</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>91</v>
@@ -1639,7 +1642,7 @@
       </c>
       <c r="W11" s="16"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>72</v>
       </c>
@@ -1700,7 +1703,7 @@
       </c>
       <c r="W12" s="16"/>
     </row>
-    <row r="13" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>72</v>
       </c>
@@ -1723,21 +1726,29 @@
         <v>9</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I13" s="6"/>
+        <v>9</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>91</v>
+      </c>
       <c r="J13" s="6" t="s">
         <v>110</v>
       </c>
       <c r="K13" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="L13" s="6"/>
+      <c r="L13" s="11" t="s">
+        <v>113</v>
+      </c>
       <c r="M13" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="N13" s="4"/>
-      <c r="O13" s="6"/>
+      <c r="N13" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="O13" s="13" t="s">
+        <v>113</v>
+      </c>
       <c r="P13" s="6"/>
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
@@ -1747,7 +1758,7 @@
       <c r="V13" s="4"/>
       <c r="W13" s="6"/>
     </row>
-    <row r="14" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>72</v>
       </c>
@@ -1770,21 +1781,29 @@
         <v>9</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I14" s="6"/>
+        <v>9</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>91</v>
+      </c>
       <c r="J14" s="6" t="s">
         <v>110</v>
       </c>
       <c r="K14" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="L14" s="6"/>
+      <c r="L14" s="11" t="s">
+        <v>113</v>
+      </c>
       <c r="M14" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="N14" s="4"/>
-      <c r="O14" s="6"/>
+      <c r="N14" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="O14" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="P14" s="6"/>
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
@@ -1794,7 +1813,7 @@
       <c r="V14" s="4"/>
       <c r="W14" s="6"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>72</v>
       </c>
@@ -1817,7 +1836,7 @@
         <v>3</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>91</v>
@@ -1859,7 +1878,7 @@
       </c>
       <c r="W15" s="16"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>73</v>
       </c>
@@ -1882,7 +1901,7 @@
         <v>3</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>91</v>
@@ -1924,7 +1943,7 @@
       </c>
       <c r="W16" s="16"/>
     </row>
-    <row r="17" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>72</v>
       </c>
@@ -1971,7 +1990,7 @@
       <c r="V17" s="4"/>
       <c r="W17" s="6"/>
     </row>
-    <row r="18" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>73</v>
       </c>
@@ -2018,7 +2037,7 @@
       <c r="V18" s="4"/>
       <c r="W18" s="6"/>
     </row>
-    <row r="19" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>73</v>
       </c>
@@ -2065,7 +2084,7 @@
       <c r="V19" s="4"/>
       <c r="W19" s="6"/>
     </row>
-    <row r="20" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>73</v>
       </c>
@@ -2112,7 +2131,7 @@
       <c r="V20" s="4"/>
       <c r="W20" s="6"/>
     </row>
-    <row r="21" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>73</v>
       </c>
@@ -2159,7 +2178,7 @@
       <c r="V21" s="4"/>
       <c r="W21" s="6"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>73</v>
       </c>
@@ -2182,7 +2201,7 @@
         <v>3</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>91</v>
@@ -2220,7 +2239,7 @@
       </c>
       <c r="W22" s="16"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>73</v>
       </c>
@@ -2281,7 +2300,7 @@
       </c>
       <c r="W23" s="16"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>73</v>
       </c>
@@ -2342,7 +2361,7 @@
       </c>
       <c r="W24" s="16"/>
     </row>
-    <row r="25" spans="1:23" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>73</v>
       </c>
@@ -2389,7 +2408,7 @@
       <c r="V25" s="4"/>
       <c r="W25" s="6"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>73</v>
       </c>
@@ -2450,7 +2469,7 @@
       </c>
       <c r="W26" s="16"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>73</v>
       </c>
@@ -2511,7 +2530,7 @@
       </c>
       <c r="W27" s="16"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>73</v>
       </c>
@@ -2572,7 +2591,7 @@
       </c>
       <c r="W28" s="16"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>73</v>
       </c>
@@ -2637,7 +2656,7 @@
       </c>
       <c r="W29" s="16"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>73</v>
       </c>
@@ -2660,7 +2679,7 @@
         <v>3</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I30" s="6" t="s">
         <v>91</v>
@@ -2702,7 +2721,7 @@
       </c>
       <c r="W30" s="16"/>
     </row>
-    <row r="31" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>73</v>
       </c>
@@ -2725,7 +2744,7 @@
         <v>9</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I31" s="6" t="s">
         <v>91</v>
@@ -2765,7 +2784,7 @@
       </c>
       <c r="W31" s="16"/>
     </row>
-    <row r="32" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>73</v>
       </c>
@@ -2812,7 +2831,7 @@
       <c r="V32" s="4"/>
       <c r="W32" s="6"/>
     </row>
-    <row r="33" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>73</v>
       </c>
@@ -2859,7 +2878,7 @@
       <c r="V33" s="4"/>
       <c r="W33" s="6"/>
     </row>
-    <row r="34" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>73</v>
       </c>
@@ -2906,7 +2925,7 @@
       <c r="V34" s="4"/>
       <c r="W34" s="6"/>
     </row>
-    <row r="35" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>73</v>
       </c>
@@ -2953,7 +2972,7 @@
       <c r="V35" s="4"/>
       <c r="W35" s="6"/>
     </row>
-    <row r="36" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>73</v>
       </c>
@@ -3000,7 +3019,7 @@
       <c r="V36" s="4"/>
       <c r="W36" s="6"/>
     </row>
-    <row r="37" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>73</v>
       </c>
@@ -3047,7 +3066,7 @@
       <c r="V37" s="4"/>
       <c r="W37" s="6"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>73</v>
       </c>
@@ -3070,7 +3089,7 @@
         <v>9</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I38" s="6" t="s">
         <v>91</v>
@@ -3108,7 +3127,7 @@
       <c r="V38" s="4"/>
       <c r="W38" s="16"/>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>72</v>
       </c>
@@ -3131,7 +3150,7 @@
         <v>9</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I39" s="6" t="s">
         <v>91</v>
@@ -3173,7 +3192,7 @@
       </c>
       <c r="W39" s="16"/>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>73</v>
       </c>
@@ -3234,7 +3253,7 @@
       </c>
       <c r="W40" s="16"/>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>73</v>
       </c>
@@ -3295,7 +3314,7 @@
       </c>
       <c r="W41" s="16"/>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>73</v>
       </c>
@@ -3356,7 +3375,7 @@
       </c>
       <c r="W42" s="16"/>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>73</v>
       </c>
@@ -3417,7 +3436,7 @@
       </c>
       <c r="W43" s="16"/>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>72</v>
       </c>
@@ -3482,7 +3501,7 @@
       </c>
       <c r="W44" s="16"/>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>73</v>
       </c>
@@ -3543,7 +3562,7 @@
       </c>
       <c r="W45" s="16"/>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>73</v>
       </c>
@@ -3604,7 +3623,7 @@
       </c>
       <c r="W46" s="16"/>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>73</v>
       </c>
@@ -3627,7 +3646,7 @@
         <v>3</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I47" s="6" t="s">
         <v>91</v>
@@ -3665,7 +3684,7 @@
       </c>
       <c r="W47" s="16"/>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>73</v>
       </c>
@@ -3726,7 +3745,7 @@
       </c>
       <c r="W48" s="16"/>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>72</v>
       </c>
@@ -3791,7 +3810,7 @@
       </c>
       <c r="W49" s="16"/>
     </row>
-    <row r="50" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>73</v>
       </c>
@@ -3838,7 +3857,7 @@
       <c r="V50" s="4"/>
       <c r="W50" s="6"/>
     </row>
-    <row r="51" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>73</v>
       </c>
@@ -3885,7 +3904,7 @@
       <c r="V51" s="4"/>
       <c r="W51" s="6"/>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>73</v>
       </c>
@@ -3946,7 +3965,7 @@
       </c>
       <c r="W52" s="16"/>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>73</v>
       </c>
@@ -4007,7 +4026,7 @@
       </c>
       <c r="W53" s="16"/>
     </row>
-    <row r="54" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>73</v>
       </c>
@@ -4054,7 +4073,7 @@
       <c r="V54" s="4"/>
       <c r="W54" s="6"/>
     </row>
-    <row r="55" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>73</v>
       </c>
@@ -4101,7 +4120,7 @@
       <c r="V55" s="4"/>
       <c r="W55" s="6"/>
     </row>
-    <row r="56" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>73</v>
       </c>
@@ -4148,7 +4167,7 @@
       <c r="V56" s="4"/>
       <c r="W56" s="6"/>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>73</v>
       </c>
@@ -4209,7 +4228,7 @@
       </c>
       <c r="W57" s="16"/>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>73</v>
       </c>
@@ -4232,7 +4251,7 @@
         <v>9</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I58" s="6" t="s">
         <v>91</v>
@@ -4274,7 +4293,7 @@
       </c>
       <c r="W58" s="16"/>
     </row>
-    <row r="59" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>73</v>
       </c>
@@ -4321,7 +4340,7 @@
       <c r="V59" s="4"/>
       <c r="W59" s="6"/>
     </row>
-    <row r="60" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>73</v>
       </c>
@@ -4368,7 +4387,7 @@
       <c r="V60" s="4"/>
       <c r="W60" s="6"/>
     </row>
-    <row r="61" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
         <v>73</v>
       </c>
@@ -4415,7 +4434,7 @@
       <c r="V61" s="4"/>
       <c r="W61" s="6"/>
     </row>
-    <row r="62" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>73</v>
       </c>
@@ -4462,7 +4481,7 @@
       <c r="V62" s="4"/>
       <c r="W62" s="6"/>
     </row>
-    <row r="63" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>73</v>
       </c>
@@ -4509,7 +4528,7 @@
       <c r="V63" s="4"/>
       <c r="W63" s="6"/>
     </row>
-    <row r="64" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>73</v>
       </c>
@@ -4556,7 +4575,7 @@
       <c r="V64" s="4"/>
       <c r="W64" s="6"/>
     </row>
-    <row r="65" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>73</v>
       </c>

</xml_diff>